<commit_message>
New report with new data
</commit_message>
<xml_diff>
--- a/FinalProject/Data/UN data/HDR21-22_Statistical_Annex_HDI_Table.xlsx
+++ b/FinalProject/Data/UN data/HDR21-22_Statistical_Annex_HDI_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admir.jahic\Desktop\HDRO\HDR 2021\Web materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dima1\OneDrive - Queen Mary, University of London\Documents\Year 2\Software Practices\ProfessionalSoftwareModule\FinalProject\Data\UN data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC8214E-DB48-44AE-871A-E2A548183FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD51D35B-6E09-47D6-AD42-883E899E3EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1965,33 +1965,33 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="12"/>
-    <col min="2" max="2" width="45.21875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="12"/>
+    <col min="2" max="2" width="45.1796875" style="12" customWidth="1"/>
     <col min="3" max="3" width="17" style="12" customWidth="1"/>
     <col min="4" max="4" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="12" customWidth="1"/>
     <col min="6" max="6" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" style="12" customWidth="1"/>
     <col min="8" max="8" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" style="12" customWidth="1"/>
     <col min="10" max="10" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" style="12" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" style="12" customWidth="1"/>
-    <col min="13" max="13" width="22.21875" style="12" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="2.81640625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="22.1796875" style="12" customWidth="1"/>
     <col min="14" max="14" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.21875" style="12" customWidth="1"/>
+    <col min="15" max="15" width="14.1796875" style="12" customWidth="1"/>
     <col min="16" max="16" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.77734375" style="12"/>
+    <col min="17" max="17" width="8.81640625" style="12"/>
     <col min="18" max="18" width="2" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.77734375" style="12"/>
+    <col min="19" max="16384" width="8.81640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="10" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>328</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="14" x14ac:dyDescent="0.25">
       <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
@@ -2016,13 +2016,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="14" x14ac:dyDescent="0.25">
       <c r="E4" s="17"/>
       <c r="G4" s="17"/>
       <c r="I4" s="17"/>
       <c r="K4" s="17"/>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="16"/>
       <c r="C5" s="17" t="s">
@@ -2054,7 +2054,7 @@
       </c>
       <c r="P5" s="16"/>
     </row>
-    <row r="6" spans="1:27" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2086,7 +2086,7 @@
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="17">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="P7" s="16"/>
     </row>
-    <row r="8" spans="1:27" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="23" t="s">
         <v>18</v>
@@ -2155,7 +2155,7 @@
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="14" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>1</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>2</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>3</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>4</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>5</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>6</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>7</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>8</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>9</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>10</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>11</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>12</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>13</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>13</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>15</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>16</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>17</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>18</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>19</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>19</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>21</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>22</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>23</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>23</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>25</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>26</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>27</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>28</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>29</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>30</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>31</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>32</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>33</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>34</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>35</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>35</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>35</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>38</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>39</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>40</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>40</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>42</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>42</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>44</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>45</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>46</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>47</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>48</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>49</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>50</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>51</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>52</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>53</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>54</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>55</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>56</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>57</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <v>58</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>58</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>60</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>61</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <v>62</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>63</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>63</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>63</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <v>66</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="23" t="s">
         <v>97</v>
@@ -4229,7 +4229,7 @@
       <c r="N75" s="23"/>
       <c r="O75" s="23"/>
     </row>
-    <row r="76" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>67</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>68</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <v>68</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>70</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>71</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>72</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>73</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>74</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <v>75</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <v>76</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <v>77</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <v>78</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <v>79</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <v>80</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <v>80</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <v>80</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <v>83</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <v>84</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <v>85</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <v>86</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <v>87</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <v>88</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <v>89</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <v>90</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <v>91</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A101" s="15">
         <v>91</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A102" s="15">
         <v>91</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A103" s="15">
         <v>91</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A104" s="15">
         <v>95</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A105" s="15">
         <v>96</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A106" s="15">
         <v>97</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A107" s="15">
         <v>97</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A108" s="15">
         <v>99</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A109" s="15">
         <v>99</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A110" s="15">
         <v>101</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A111" s="15">
         <v>102</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A112" s="15">
         <v>102</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A113" s="15">
         <v>104</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A114" s="15">
         <v>105</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A115" s="15">
         <v>106</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A116" s="15">
         <v>106</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A117" s="15">
         <v>108</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A118" s="15">
         <v>109</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A119" s="15">
         <v>110</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A120" s="15">
         <v>111</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A121" s="15">
         <v>112</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A122" s="15">
         <v>112</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A123" s="15">
         <v>114</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A124" s="15">
         <v>115</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:15" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="23" t="s">
         <v>153</v>
@@ -5822,7 +5822,7 @@
       <c r="N125" s="23"/>
       <c r="O125" s="23"/>
     </row>
-    <row r="126" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A126" s="15">
         <v>116</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="15">
         <v>117</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A128" s="15">
         <v>118</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A129" s="15">
         <v>118</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A130" s="15">
         <v>120</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A131" s="15">
         <v>121</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="15">
         <v>122</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A133" s="15">
         <v>123</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A134" s="15">
         <v>123</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A135" s="15">
         <v>125</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A136" s="15">
         <v>126</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A137" s="15">
         <v>127</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="15">
         <v>128</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A139" s="15">
         <v>129</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A140" s="15">
         <v>130</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A141" s="15">
         <v>131</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A142" s="15">
         <v>132</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A143" s="15">
         <v>133</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A144" s="15">
         <v>134</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A145" s="15">
         <v>135</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A146" s="15">
         <v>136</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A147" s="15">
         <v>137</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A148" s="15">
         <v>138</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A149" s="15">
         <v>139</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A150" s="15">
         <v>140</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A151" s="15">
         <v>140</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A152" s="15">
         <v>140</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A153" s="15">
         <v>143</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A154" s="15">
         <v>144</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A155" s="15">
         <v>145</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A156" s="15">
         <v>146</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A157" s="15">
         <v>146</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A158" s="15">
         <v>148</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A159" s="15">
         <v>149</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A160" s="15">
         <v>150</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A161" s="15">
         <v>151</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A162" s="15">
         <v>152</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A163" s="15">
         <v>153</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A164" s="15">
         <v>154</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="15">
         <v>155</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A166" s="15">
         <v>156</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A167" s="15">
         <v>156</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A168" s="15">
         <v>158</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A169" s="15">
         <v>159</v>
       </c>
@@ -7251,7 +7251,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="170" spans="1:15" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A170" s="6"/>
       <c r="B170" s="23" t="s">
         <v>203</v>
@@ -7270,7 +7270,7 @@
       <c r="N170" s="23"/>
       <c r="O170" s="23"/>
     </row>
-    <row r="171" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="15">
         <v>160</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A172" s="15">
         <v>161</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A173" s="15">
         <v>162</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A174" s="15">
         <v>163</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A175" s="15">
         <v>163</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A176" s="15">
         <v>165</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A177" s="15">
         <v>166</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A178" s="15">
         <v>166</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A179" s="15">
         <v>168</v>
       </c>
@@ -7567,7 +7567,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A180" s="15">
         <v>169</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A181" s="15">
         <v>170</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A182" s="15">
         <v>171</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A183" s="15">
         <v>172</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A184" s="15">
         <v>173</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A185" s="15">
         <v>174</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A186" s="15">
         <v>175</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A187" s="15">
         <v>176</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A188" s="15">
         <v>177</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="14" x14ac:dyDescent="0.25">
       <c r="A189" s="15">
         <v>178</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="15">
         <v>179</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A191" s="15">
         <v>180</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A192" s="15">
         <v>181</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A193" s="15">
         <v>182</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A194" s="15">
         <v>183</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A195" s="15">
         <v>184</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A196" s="15">
         <v>185</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A197" s="15">
         <v>186</v>
       </c>
@@ -8167,7 +8167,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="198" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A198" s="15">
         <v>187</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="199" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A199" s="15">
         <v>188</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A200" s="15">
         <v>189</v>
       </c>
@@ -8269,7 +8269,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="201" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A201" s="15">
         <v>190</v>
       </c>
@@ -8304,7 +8304,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A202" s="15">
         <v>191</v>
       </c>
@@ -8339,7 +8339,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="203" spans="1:17" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A203" s="6"/>
       <c r="B203" s="23" t="s">
         <v>239</v>
@@ -8358,7 +8358,7 @@
       <c r="N203" s="23"/>
       <c r="O203" s="23"/>
     </row>
-    <row r="204" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B204" s="10" t="s">
         <v>240</v>
       </c>
@@ -8388,7 +8388,7 @@
       </c>
       <c r="Q204" s="6"/>
     </row>
-    <row r="205" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B205" s="10" t="s">
         <v>242</v>
       </c>
@@ -8415,7 +8415,7 @@
       </c>
       <c r="Q205" s="6"/>
     </row>
-    <row r="206" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B206" s="10" t="s">
         <v>243</v>
       </c>
@@ -8445,7 +8445,7 @@
       </c>
       <c r="Q206" s="6"/>
     </row>
-    <row r="207" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B207" s="10" t="s">
         <v>244</v>
       </c>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="Q207" s="6"/>
     </row>
-    <row r="208" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B208" s="10"/>
       <c r="C208" s="6"/>
       <c r="E208" s="14"/>
@@ -8483,13 +8483,13 @@
       <c r="O208" s="6"/>
       <c r="Q208" s="6"/>
     </row>
-    <row r="209" spans="1:17" s="5" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A209" s="8"/>
       <c r="B209" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B210" s="10" t="s">
         <v>246</v>
       </c>
@@ -8516,7 +8516,7 @@
       </c>
       <c r="Q210" s="6"/>
     </row>
-    <row r="211" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B211" s="10" t="s">
         <v>248</v>
       </c>
@@ -8543,7 +8543,7 @@
       </c>
       <c r="Q211" s="6"/>
     </row>
-    <row r="212" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B212" s="10" t="s">
         <v>249</v>
       </c>
@@ -8570,7 +8570,7 @@
       </c>
       <c r="Q212" s="6"/>
     </row>
-    <row r="213" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B213" s="10" t="s">
         <v>250</v>
       </c>
@@ -8597,7 +8597,7 @@
       </c>
       <c r="Q213" s="6"/>
     </row>
-    <row r="214" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B214" s="10"/>
       <c r="C214" s="13"/>
       <c r="E214" s="14"/>
@@ -8608,7 +8608,7 @@
       <c r="O214" s="6"/>
       <c r="Q214" s="6"/>
     </row>
-    <row r="215" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B215" s="9" t="s">
         <v>251</v>
       </c>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="Q215" s="6"/>
     </row>
-    <row r="216" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B216" s="9"/>
       <c r="C216" s="13"/>
       <c r="E216" s="14"/>
@@ -8646,7 +8646,7 @@
       <c r="O216" s="6"/>
       <c r="Q216" s="6"/>
     </row>
-    <row r="217" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B217" s="1" t="s">
         <v>252</v>
       </c>
@@ -8659,7 +8659,7 @@
       <c r="O217" s="6"/>
       <c r="Q217" s="6"/>
     </row>
-    <row r="218" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B218" s="10" t="s">
         <v>253</v>
       </c>
@@ -8686,7 +8686,7 @@
       </c>
       <c r="Q218" s="6"/>
     </row>
-    <row r="219" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B219" s="10" t="s">
         <v>254</v>
       </c>
@@ -8713,7 +8713,7 @@
       </c>
       <c r="Q219" s="6"/>
     </row>
-    <row r="220" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B220" s="10" t="s">
         <v>255</v>
       </c>
@@ -8740,7 +8740,7 @@
       </c>
       <c r="Q220" s="6"/>
     </row>
-    <row r="221" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B221" s="10" t="s">
         <v>256</v>
       </c>
@@ -8767,7 +8767,7 @@
       </c>
       <c r="Q221" s="6"/>
     </row>
-    <row r="222" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B222" s="10" t="s">
         <v>257</v>
       </c>
@@ -8794,7 +8794,7 @@
       </c>
       <c r="Q222" s="6"/>
     </row>
-    <row r="223" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B223" s="10" t="s">
         <v>258</v>
       </c>
@@ -8821,7 +8821,7 @@
       </c>
       <c r="Q223" s="6"/>
     </row>
-    <row r="224" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B224" s="10"/>
       <c r="C224" s="13"/>
       <c r="E224" s="14"/>
@@ -8832,7 +8832,7 @@
       <c r="O224" s="6"/>
       <c r="Q224" s="6"/>
     </row>
-    <row r="225" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B225" s="9" t="s">
         <v>259</v>
       </c>
@@ -8859,7 +8859,7 @@
       </c>
       <c r="Q225" s="6"/>
     </row>
-    <row r="226" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B226" s="1" t="s">
         <v>260</v>
       </c>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="Q226" s="6"/>
     </row>
-    <row r="227" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
       <c r="C227" s="13"/>
       <c r="E227" s="14"/>
@@ -8897,7 +8897,7 @@
       <c r="O227" s="6"/>
       <c r="Q227" s="6"/>
     </row>
-    <row r="228" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B228" s="1" t="s">
         <v>261</v>
       </c>
@@ -8924,7 +8924,7 @@
       </c>
       <c r="Q228" s="6"/>
     </row>
-    <row r="229" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
       <c r="C229" s="13"/>
       <c r="E229" s="14"/>
@@ -8935,7 +8935,7 @@
       <c r="O229" s="6"/>
       <c r="Q229" s="6"/>
     </row>
-    <row r="230" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B230" s="9" t="s">
         <v>262</v>
       </c>
@@ -8962,87 +8962,87 @@
       </c>
       <c r="Q230" s="6"/>
     </row>
-    <row r="232" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B232" s="9" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="233" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B233" s="10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="234" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B234" s="10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="235" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B235" s="10" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="236" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B236" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="237" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B237" s="10" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="238" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B238" s="10" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="239" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B239" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="240" spans="2:17" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:17" ht="14" x14ac:dyDescent="0.25">
       <c r="B240" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="241" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B241" s="10" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="242" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B242" s="10" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="243" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B243" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="244" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B244" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="245" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B245" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="246" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B246" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="247" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B247" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="248" spans="2:13" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:13" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="B248" s="10" t="s">
         <v>292</v>
       </c>
@@ -9058,7 +9058,7 @@
       <c r="L248" s="10"/>
       <c r="M248" s="10"/>
     </row>
-    <row r="249" spans="2:13" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:13" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="B249" s="10" t="s">
         <v>293</v>
       </c>
@@ -9074,7 +9074,7 @@
       <c r="L249" s="10"/>
       <c r="M249" s="10"/>
     </row>
-    <row r="250" spans="2:13" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:13" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="B250" s="10" t="s">
         <v>294</v>
       </c>
@@ -9090,122 +9090,122 @@
       <c r="L250" s="10"/>
       <c r="M250" s="10"/>
     </row>
-    <row r="251" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B251" s="10" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="252" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B252" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="253" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B253" s="10" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="254" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B254" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="255" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B255" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="256" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:13" ht="14" x14ac:dyDescent="0.25">
       <c r="B256" s="10" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="257" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B257" s="10" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="258" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B258" s="10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="259" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B259" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="262" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B262" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="263" spans="2:2" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B263" s="10" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="264" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B264" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="265" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B265" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="266" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B266" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="267" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B267" s="10" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="268" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B268" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="269" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B269" s="10" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="271" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B271" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B272" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="273" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B273" s="10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="274" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B274" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B275" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B276" s="10" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" ht="14" x14ac:dyDescent="0.25">
       <c r="B277" s="10" t="s">
         <v>276</v>
       </c>
@@ -9232,14 +9232,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F18D9B4-E7DC-4119-BC32-968206E6CA59}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="166.88671875" style="12" customWidth="1"/>
-    <col min="2" max="16384" width="8.77734375" style="12"/>
+    <col min="1" max="1" width="166.90625" style="12" customWidth="1"/>
+    <col min="2" max="16384" width="8.81640625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -9247,125 +9247,125 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
     </row>
-    <row r="5" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>321</v>
       </c>
@@ -9379,17 +9379,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="7f64e6aa-b736-4f26-84cc-faf427629e48">
-      <UserInfo>
-        <DisplayName>Cecilia Calderon</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9572,20 +9567,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="7f64e6aa-b736-4f26-84cc-faf427629e48">
+      <UserInfo>
+        <DisplayName>Cecilia Calderon</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7DA61EB-8D48-4617-94E1-454D1449F940}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BAEA50D-A77A-4BD1-A57D-FE81CA4DEB01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f64e6aa-b736-4f26-84cc-faf427629e48"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9610,9 +9608,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BAEA50D-A77A-4BD1-A57D-FE81CA4DEB01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7DA61EB-8D48-4617-94E1-454D1449F940}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f64e6aa-b736-4f26-84cc-faf427629e48"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>